<commit_message>
Modificación envio de imagenes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -48,7 +48,7 @@
     <t xml:space="preserve">pathImages</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\Users\diana.ciro\Desktop\SUAM\imagenesUipath\report</t>
+    <t xml:space="preserve">../Captures</t>
   </si>
   <si>
     <t xml:space="preserve">receivers</t>
@@ -318,7 +318,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>